<commit_message>
Update table ProgramariConsultatii in NF1
</commit_message>
<xml_diff>
--- a/PS/DatabaseDesign/tabele.xlsx
+++ b/PS/DatabaseDesign/tabele.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="13140"/>
+    <workbookView windowWidth="22943" windowHeight="10871"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75">
   <si>
     <t>Incasari</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>ora_programare</t>
+  </si>
+  <si>
+    <t>minut_programare</t>
   </si>
   <si>
     <t>FoiConsultatie</t>
@@ -245,9 +248,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="29">
@@ -331,17 +334,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,6 +356,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -362,9 +379,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -385,86 +418,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -484,19 +487,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,163 +619,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,6 +678,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -697,7 +724,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -713,36 +740,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -767,11 +764,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,156 +783,153 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -962,54 +962,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
-    <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
-    <cellStyle name="Accent5" xfId="6" builtinId="45"/>
-    <cellStyle name="Percent" xfId="7" builtinId="5"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Accent4" xfId="9" builtinId="41"/>
-    <cellStyle name="60% - Accent3" xfId="10" builtinId="40"/>
-    <cellStyle name="20% - Accent3" xfId="11" builtinId="38"/>
-    <cellStyle name="Accent3" xfId="12" builtinId="37"/>
-    <cellStyle name="20% - Accent2" xfId="13" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="14" builtinId="33"/>
-    <cellStyle name="Accent6" xfId="15" builtinId="49"/>
-    <cellStyle name="60% - Accent1" xfId="16" builtinId="32"/>
-    <cellStyle name="Heading 4" xfId="17" builtinId="19"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="40% - Accent4" xfId="19" builtinId="43"/>
-    <cellStyle name="40% - Accent3" xfId="20" builtinId="39"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="Bad" xfId="22" builtinId="27"/>
-    <cellStyle name="Linked Cell" xfId="23" builtinId="24"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Note" xfId="27" builtinId="10"/>
-    <cellStyle name="Input" xfId="28" builtinId="20"/>
-    <cellStyle name="Good" xfId="29" builtinId="26"/>
-    <cellStyle name="60% - Accent2" xfId="30" builtinId="36"/>
-    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18"/>
-    <cellStyle name="Heading 1" xfId="33" builtinId="16"/>
-    <cellStyle name="60% - Accent6" xfId="34" builtinId="52"/>
-    <cellStyle name="20% - Accent1" xfId="35" builtinId="30"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="40% - Accent2" xfId="38" builtinId="35"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Accent1" xfId="40" builtinId="29"/>
-    <cellStyle name="CExplanatory Text" xfId="41" builtinId="53"/>
-    <cellStyle name="Currency" xfId="42" builtinId="4"/>
-    <cellStyle name="Warning Text" xfId="43" builtinId="11"/>
-    <cellStyle name="Currency [0]" xfId="44" builtinId="7"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1310,34 +1310,34 @@
   <dimension ref="A3:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="15.8" customWidth="1"/>
-    <col min="3" max="3" width="16.6" customWidth="1"/>
-    <col min="4" max="4" width="16.4" customWidth="1"/>
-    <col min="5" max="5" width="18.4" customWidth="1"/>
+    <col min="2" max="2" width="15.7962962962963" customWidth="1"/>
+    <col min="3" max="3" width="16.6018518518519" customWidth="1"/>
+    <col min="4" max="4" width="16.3981481481481" customWidth="1"/>
+    <col min="5" max="5" width="18.3981481481481" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.4" customWidth="1"/>
-    <col min="8" max="8" width="13.6" customWidth="1"/>
+    <col min="7" max="7" width="18.3981481481481" customWidth="1"/>
+    <col min="8" max="8" width="16.5555555555556" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="13.6" customWidth="1"/>
-    <col min="12" max="12" width="15.7" customWidth="1"/>
-    <col min="13" max="13" width="12.1" customWidth="1"/>
-    <col min="14" max="14" width="12.9" customWidth="1"/>
-    <col min="15" max="15" width="10.6" customWidth="1"/>
-    <col min="16" max="16" width="12.2" customWidth="1"/>
+    <col min="11" max="11" width="13.6018518518519" customWidth="1"/>
+    <col min="12" max="12" width="15.7037037037037" customWidth="1"/>
+    <col min="13" max="13" width="12.1018518518519" customWidth="1"/>
+    <col min="14" max="14" width="12.8981481481481" customWidth="1"/>
+    <col min="15" max="15" width="10.6018518518519" customWidth="1"/>
+    <col min="16" max="16" width="12.2037037037037" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="13.3" customWidth="1"/>
+    <col min="18" max="18" width="13.2962962962963" customWidth="1"/>
     <col min="19" max="20" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1403,16 +1403,16 @@
       <c r="K8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="N8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -1435,7 +1435,7 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="M10" s="1"/>
@@ -1459,11 +1459,11 @@
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:8">
+    <row r="16" s="1" customFormat="1" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1486,26 +1486,29 @@
         <v>39</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="7" t="s">
-        <v>40</v>
+      <c r="A18" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>2</v>
@@ -1514,39 +1517,39 @@
         <v>10</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="8" t="s">
-        <v>47</v>
+      <c r="A21" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="9" t="s">
-        <v>52</v>
+      <c r="A24" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>2</v>
@@ -1555,38 +1558,38 @@
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="10" t="s">
-        <v>58</v>
+      <c r="A27" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="1" spans="1:17">
+    <row r="28" s="1" customFormat="1" spans="1:17">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>2</v>
@@ -1595,38 +1598,38 @@
         <v>3</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="N28" s="2" t="s">
+      <c r="M28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O28" s="2" t="s">
+      <c r="N28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="O28" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="P28" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="Q28" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
@@ -1641,9 +1644,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
@@ -1658,9 +1661,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
remove ids as primary keys
</commit_message>
<xml_diff>
--- a/PS/DatabaseDesign/tabele.xlsx
+++ b/PS/DatabaseDesign/tabele.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="10871"/>
+    <workbookView windowWidth="22935" windowHeight="10830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67">
   <si>
     <t>Incasari</t>
   </si>
   <si>
-    <t>id_incasare (PrimaryKey)</t>
-  </si>
-  <si>
     <t>nume_pacient</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t xml:space="preserve">Medici </t>
   </si>
   <si>
-    <t>id_medic (PrimaryKey)</t>
-  </si>
-  <si>
     <t>nume_medic</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>PlatiMedici</t>
   </si>
   <si>
-    <t>id_plata (PrimaryKey)</t>
-  </si>
-  <si>
     <t>bonus</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>ProgramariConsultatii</t>
   </si>
   <si>
-    <t>id_programare (PrimaryKey)</t>
-  </si>
-  <si>
     <t>zi_programare</t>
   </si>
   <si>
@@ -144,9 +132,6 @@
     <t>FoiConsultatie</t>
   </si>
   <si>
-    <t>id_consultatie (PrimaryKey)</t>
-  </si>
-  <si>
     <t>zi_consultatie</t>
   </si>
   <si>
@@ -165,9 +150,6 @@
     <t>CatalogInterventii</t>
   </si>
   <si>
-    <t>id_interventie (PrimaryKey)</t>
-  </si>
-  <si>
     <t>tip_interventie</t>
   </si>
   <si>
@@ -180,9 +162,6 @@
     <t>Chitante</t>
   </si>
   <si>
-    <t>id_chitanta (PrimaryKey)</t>
-  </si>
-  <si>
     <t>zi_chitanta</t>
   </si>
   <si>
@@ -196,9 +175,6 @@
   </si>
   <si>
     <t>FisePacienti</t>
-  </si>
-  <si>
-    <t>id_fisa (PrimaryKey)</t>
   </si>
   <si>
     <t>numar_fisa</t>
@@ -248,10 +224,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -335,7 +311,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -379,6 +362,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -404,7 +401,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,7 +432,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -435,44 +440,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -487,19 +463,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,163 +583,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,6 +654,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -720,15 +705,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -758,8 +734,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -783,7 +759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -801,130 +777,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1307,33 +1283,33 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:U28"/>
+  <dimension ref="A3:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="15.7962962962963" customWidth="1"/>
-    <col min="3" max="3" width="16.6018518518519" customWidth="1"/>
-    <col min="4" max="4" width="16.3981481481481" customWidth="1"/>
-    <col min="5" max="5" width="18.3981481481481" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.3981481481481" customWidth="1"/>
-    <col min="8" max="8" width="16.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="15.8" customWidth="1"/>
+    <col min="3" max="3" width="16.6" customWidth="1"/>
+    <col min="4" max="4" width="16.4" customWidth="1"/>
+    <col min="5" max="5" width="18.4" customWidth="1"/>
+    <col min="6" max="6" width="13.5047619047619" customWidth="1"/>
+    <col min="7" max="7" width="18.4" customWidth="1"/>
+    <col min="8" max="8" width="16.552380952381" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="13.6018518518519" customWidth="1"/>
-    <col min="12" max="12" width="15.7037037037037" customWidth="1"/>
-    <col min="13" max="13" width="12.1018518518519" customWidth="1"/>
-    <col min="14" max="14" width="12.8981481481481" customWidth="1"/>
-    <col min="15" max="15" width="10.6018518518519" customWidth="1"/>
-    <col min="16" max="16" width="12.2037037037037" customWidth="1"/>
+    <col min="11" max="11" width="13.6" customWidth="1"/>
+    <col min="12" max="12" width="15.7047619047619" customWidth="1"/>
+    <col min="13" max="13" width="12.1047619047619" customWidth="1"/>
+    <col min="14" max="14" width="12.8952380952381" customWidth="1"/>
+    <col min="15" max="15" width="10.6" customWidth="1"/>
+    <col min="16" max="16" width="12.2" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="13.2962962962963" customWidth="1"/>
-    <col min="19" max="20" width="13.5" customWidth="1"/>
+    <col min="18" max="18" width="13.2952380952381" customWidth="1"/>
+    <col min="19" max="20" width="13.5047619047619" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1">
@@ -1341,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:7">
+    <row r="4" s="1" customFormat="1" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1359,273 +1335,249 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:20">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:21">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:5">
+    <row r="11" s="1" customFormat="1" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:9">
+    <row r="16" s="1" customFormat="1" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:7">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="1:8">
-      <c r="A19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="1" spans="1:4">
+    <row r="22" s="1" customFormat="1" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="1" spans="1:7">
+    <row r="25" s="1" customFormat="1" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="28" s="1" customFormat="1" spans="1:17">
+    <row r="28" s="1" customFormat="1" spans="1:16">
       <c r="A28" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1644,7 +1596,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1661,7 +1613,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Tipuri de date pentru fiecare coloana
</commit_message>
<xml_diff>
--- a/PS/DatabaseDesign/tabele.xlsx
+++ b/PS/DatabaseDesign/tabele.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="112">
   <si>
     <t>Incasari 2NF</t>
   </si>
@@ -73,73 +73,76 @@
     <t>VARCHAR(25)</t>
   </si>
   <si>
+    <t>CHAR(2)</t>
+  </si>
+  <si>
+    <t>CHAR(4)</t>
+  </si>
+  <si>
+    <t>ContracteMedici</t>
+  </si>
+  <si>
+    <t>id_contract(PK)</t>
+  </si>
+  <si>
+    <t>telefon_medic</t>
+  </si>
+  <si>
+    <t>email_medic</t>
+  </si>
+  <si>
+    <t>ziua_angajarii</t>
+  </si>
+  <si>
+    <t>luna_angajarii</t>
+  </si>
+  <si>
+    <t>anul_angajarii</t>
+  </si>
+  <si>
+    <t>salariu_angajare</t>
+  </si>
+  <si>
+    <t>cnp_medic (FK)</t>
+  </si>
+  <si>
+    <t>INT(10) UNSIGNED</t>
+  </si>
+  <si>
+    <t>VARCHAR(35)</t>
+  </si>
+  <si>
+    <t>INT(13) UNSIGNED</t>
+  </si>
+  <si>
+    <t>AdreseMedici 2NF</t>
+  </si>
+  <si>
+    <t>serieci_medic</t>
+  </si>
+  <si>
+    <t>nrci_medic</t>
+  </si>
+  <si>
+    <t>strada_medic</t>
+  </si>
+  <si>
+    <t>nrstr_medic</t>
+  </si>
+  <si>
+    <t>bloc_medic</t>
+  </si>
+  <si>
+    <t>scara medic</t>
+  </si>
+  <si>
+    <t>ap_medic</t>
+  </si>
+  <si>
+    <t>oras_medic</t>
+  </si>
+  <si>
     <t>INT(2) UNSIGNED</t>
-  </si>
-  <si>
-    <t>INT(4) UNSIGNED</t>
-  </si>
-  <si>
-    <t>ContracteMedici</t>
-  </si>
-  <si>
-    <t>id_contract(PK)</t>
-  </si>
-  <si>
-    <t>telefon_medic</t>
-  </si>
-  <si>
-    <t>email_medic</t>
-  </si>
-  <si>
-    <t>ziua_angajarii</t>
-  </si>
-  <si>
-    <t>luna_angajarii</t>
-  </si>
-  <si>
-    <t>anul_angajarii</t>
-  </si>
-  <si>
-    <t>salariu_angajare</t>
-  </si>
-  <si>
-    <t>cnp_medic (FK)</t>
-  </si>
-  <si>
-    <t>INT(10) UNSIGNED</t>
-  </si>
-  <si>
-    <t>VARCHAR(35)</t>
-  </si>
-  <si>
-    <t>INT(13) UNSIGNED</t>
-  </si>
-  <si>
-    <t>AdreseMedici 2NF</t>
-  </si>
-  <si>
-    <t>serieci_medic</t>
-  </si>
-  <si>
-    <t>nrci_medic</t>
-  </si>
-  <si>
-    <t>strada_medic</t>
-  </si>
-  <si>
-    <t>nrstr_medic</t>
-  </si>
-  <si>
-    <t>bloc_medic</t>
-  </si>
-  <si>
-    <t>scara medic</t>
-  </si>
-  <si>
-    <t>ap_medic</t>
-  </si>
-  <si>
-    <t>oras_medic</t>
   </si>
   <si>
     <t>INT(6) UNSIGNED</t>
@@ -1425,7 +1428,7 @@
   <dimension ref="A3:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1623,28 +1626,28 @@
     </row>
     <row r="19" s="10" customFormat="1" spans="1:9">
       <c r="A19" s="10" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I19" s="11" t="s">
         <v>31</v>
@@ -1652,26 +1655,26 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1693,33 +1696,33 @@
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" spans="1:7">
@@ -1747,27 +1750,27 @@
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" spans="1:6">
@@ -1775,14 +1778,14 @@
         <v>5</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1790,23 +1793,23 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -1817,51 +1820,51 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="1" spans="1:14">
       <c r="A38" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -1887,19 +1890,19 @@
         <v>30</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M39" s="10" t="s">
         <v>29</v>
@@ -1947,32 +1950,32 @@
   <sheetData>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:20">
@@ -1992,7 +1995,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>33</v>
@@ -2039,7 +2042,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -2052,38 +2055,38 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>11</v>
@@ -2091,126 +2094,126 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" spans="1:16">
       <c r="A28" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the database tables definition
</commit_message>
<xml_diff>
--- a/PS/DatabaseDesign/tabele.xlsx
+++ b/PS/DatabaseDesign/tabele.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="13140"/>
+    <workbookView windowWidth="22935" windowHeight="10830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111">
   <si>
     <t>incasari OK</t>
   </si>
@@ -357,10 +357,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -443,9 +443,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -468,12 +481,50 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -481,10 +532,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -496,84 +572,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -596,13 +596,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,169 +668,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -787,21 +787,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -832,8 +817,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -849,6 +834,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -870,20 +881,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -892,152 +892,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1066,9 +1066,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1077,54 +1074,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
-    <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
-    <cellStyle name="Accent5" xfId="6" builtinId="45"/>
-    <cellStyle name="Percent" xfId="7" builtinId="5"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Accent4" xfId="9" builtinId="41"/>
-    <cellStyle name="60% - Accent3" xfId="10" builtinId="40"/>
-    <cellStyle name="20% - Accent3" xfId="11" builtinId="38"/>
-    <cellStyle name="Accent3" xfId="12" builtinId="37"/>
-    <cellStyle name="20% - Accent2" xfId="13" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="14" builtinId="33"/>
-    <cellStyle name="Accent6" xfId="15" builtinId="49"/>
-    <cellStyle name="60% - Accent1" xfId="16" builtinId="32"/>
-    <cellStyle name="Heading 4" xfId="17" builtinId="19"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="40% - Accent4" xfId="19" builtinId="43"/>
-    <cellStyle name="40% - Accent3" xfId="20" builtinId="39"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="Bad" xfId="22" builtinId="27"/>
-    <cellStyle name="Linked Cell" xfId="23" builtinId="24"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Note" xfId="27" builtinId="10"/>
-    <cellStyle name="Input" xfId="28" builtinId="20"/>
-    <cellStyle name="Good" xfId="29" builtinId="26"/>
-    <cellStyle name="60% - Accent2" xfId="30" builtinId="36"/>
-    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18"/>
-    <cellStyle name="Heading 1" xfId="33" builtinId="16"/>
-    <cellStyle name="60% - Accent6" xfId="34" builtinId="52"/>
-    <cellStyle name="20% - Accent1" xfId="35" builtinId="30"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="40% - Accent2" xfId="38" builtinId="35"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Accent1" xfId="40" builtinId="29"/>
-    <cellStyle name="CExplanatory Text" xfId="41" builtinId="53"/>
-    <cellStyle name="Currency" xfId="42" builtinId="4"/>
-    <cellStyle name="Warning Text" xfId="43" builtinId="11"/>
-    <cellStyle name="Currency [0]" xfId="44" builtinId="7"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1424,30 +1421,30 @@
   <sheetPr/>
   <dimension ref="A3:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.9" customWidth="1"/>
+    <col min="1" max="1" width="49.9047619047619" customWidth="1"/>
     <col min="2" max="2" width="15.8" customWidth="1"/>
     <col min="3" max="3" width="40.6" customWidth="1"/>
     <col min="4" max="4" width="18.6" customWidth="1"/>
-    <col min="5" max="6" width="19.14" customWidth="1"/>
-    <col min="7" max="7" width="16.14" customWidth="1"/>
-    <col min="8" max="8" width="13.5733333333333" customWidth="1"/>
+    <col min="5" max="6" width="19.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="16.1428571428571" customWidth="1"/>
+    <col min="8" max="8" width="13.5714285714286" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="14.2" customWidth="1"/>
     <col min="11" max="11" width="12.8" customWidth="1"/>
-    <col min="12" max="12" width="13.14" customWidth="1"/>
-    <col min="13" max="13" width="15.9" customWidth="1"/>
-    <col min="14" max="14" width="11.86" customWidth="1"/>
-    <col min="15" max="15" width="15.14" customWidth="1"/>
-    <col min="16" max="16" width="13.4266666666667" customWidth="1"/>
-    <col min="17" max="17" width="14.14" customWidth="1"/>
-    <col min="18" max="19" width="14.4266666666667" customWidth="1"/>
-    <col min="20" max="20" width="16.7133333333333" customWidth="1"/>
+    <col min="12" max="12" width="13.1428571428571" customWidth="1"/>
+    <col min="13" max="13" width="15.8952380952381" customWidth="1"/>
+    <col min="14" max="14" width="11.8571428571429" customWidth="1"/>
+    <col min="15" max="15" width="15.1428571428571" customWidth="1"/>
+    <col min="16" max="16" width="13.4285714285714" customWidth="1"/>
+    <col min="17" max="17" width="14.1428571428571" customWidth="1"/>
+    <col min="18" max="19" width="14.4285714285714" customWidth="1"/>
+    <col min="20" max="20" width="16.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1">
@@ -1646,7 +1643,7 @@
       <c r="H19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1924,25 +1921,25 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="15.8" customWidth="1"/>
     <col min="3" max="3" width="16.6" customWidth="1"/>
     <col min="4" max="4" width="16.4" customWidth="1"/>
     <col min="5" max="7" width="18.4" customWidth="1"/>
-    <col min="8" max="8" width="16.5533333333333" customWidth="1"/>
+    <col min="8" max="8" width="16.552380952381" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="11" max="11" width="13.6" customWidth="1"/>
-    <col min="12" max="12" width="15.7066666666667" customWidth="1"/>
-    <col min="13" max="13" width="12.1066666666667" customWidth="1"/>
-    <col min="14" max="14" width="12.8933333333333" customWidth="1"/>
+    <col min="12" max="12" width="15.7047619047619" customWidth="1"/>
+    <col min="13" max="13" width="12.1047619047619" customWidth="1"/>
+    <col min="14" max="14" width="12.8952380952381" customWidth="1"/>
     <col min="15" max="15" width="10.6" customWidth="1"/>
     <col min="16" max="16" width="12.2" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="13.2933333333333" customWidth="1"/>
-    <col min="19" max="20" width="13.5066666666667" customWidth="1"/>
+    <col min="18" max="18" width="13.2952380952381" customWidth="1"/>
+    <col min="19" max="20" width="13.5047619047619" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1">
@@ -2229,7 +2226,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2246,7 +2243,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>